<commit_message>
Mas y mas mapa
</commit_message>
<xml_diff>
--- a/src/docs/Coordenadas.xlsx
+++ b/src/docs/Coordenadas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Datos\Personal\Godot\proyectos\adventure-game\src\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90DF0DB5-26DE-4C61-B812-F0FC4C9C3C4F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1341C0D6-6644-4AE9-8B94-44A40FC8FB3E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{573FC50C-C254-42E2-B786-1F305B1EAED5}"/>
   </bookViews>
@@ -496,8 +496,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -513,7 +521,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -521,13 +529,32 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -842,500 +869,497 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9BD677B-0033-4C95-8B89-8AE02173E849}">
-  <dimension ref="A1:Q11"/>
+  <dimension ref="A1:W11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:L9"/>
+      <selection activeCell="Q9" sqref="A1:Q9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="10" width="3.26953125" bestFit="1" customWidth="1"/>
-    <col min="11" max="17" width="4.26953125" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="4.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="3" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="J2" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="K2" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="L2" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="M2" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="N2" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="O2" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="P2" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="Q2" s="3" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="I3" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="J3" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="K3" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="L3" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="M3" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="N3" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="O3" s="1" t="s">
+      <c r="O3" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="P3" s="1" t="s">
+      <c r="P3" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="Q3" s="1" t="s">
+      <c r="Q3" s="3" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="I4" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="J4" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="K4" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="L4" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="M4" s="1" t="s">
+      <c r="M4" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="N4" s="1" t="s">
+      <c r="N4" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="O4" s="1" t="s">
+      <c r="O4" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="P4" s="1" t="s">
+      <c r="P4" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="Q4" s="1" t="s">
+      <c r="Q4" s="3" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="G5" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="H5" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="I5" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="J5" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="K5" s="1" t="s">
+      <c r="K5" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="L5" s="1" t="s">
+      <c r="L5" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="M5" s="1" t="s">
+      <c r="M5" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="N5" s="1" t="s">
+      <c r="N5" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="O5" s="1" t="s">
+      <c r="O5" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="P5" s="1" t="s">
+      <c r="P5" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="Q5" s="1" t="s">
+      <c r="Q5" s="3" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F6" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="G6" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="H6" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="I6" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="J6" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="K6" s="1" t="s">
+      <c r="K6" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="L6" s="1" t="s">
+      <c r="L6" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="M6" s="1" t="s">
+      <c r="M6" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="N6" s="1" t="s">
+      <c r="N6" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="O6" s="1" t="s">
+      <c r="O6" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="P6" s="1" t="s">
+      <c r="P6" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="Q6" s="1" t="s">
+      <c r="Q6" s="3" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="G7" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="H7" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="I7" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="J7" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="K7" s="1" t="s">
+      <c r="K7" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="L7" s="1" t="s">
+      <c r="L7" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="M7" s="1" t="s">
+      <c r="M7" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="N7" s="1" t="s">
+      <c r="N7" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="O7" s="1" t="s">
+      <c r="O7" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="P7" s="1" t="s">
+      <c r="P7" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="Q7" s="1" t="s">
+      <c r="Q7" s="3" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A8" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F8" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="G8" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="H8" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="I8" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="J8" s="1" t="s">
+      <c r="J8" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="K8" s="1" t="s">
+      <c r="K8" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="L8" s="1" t="s">
+      <c r="L8" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="M8" s="1" t="s">
+      <c r="M8" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="N8" s="1" t="s">
+      <c r="N8" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="O8" s="1" t="s">
+      <c r="O8" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="P8" s="1" t="s">
+      <c r="P8" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="Q8" s="1" t="s">
+      <c r="Q8" s="3" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="s">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A9" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F9" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="G9" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="H9" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="I9" s="1" t="s">
+      <c r="I9" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="J9" s="1" t="s">
+      <c r="J9" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="K9" s="1" t="s">
+      <c r="K9" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="L9" s="1" t="s">
+      <c r="L9" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="M9" s="1" t="s">
+      <c r="M9" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="N9" s="1" t="s">
+      <c r="N9" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="O9" s="1" t="s">
+      <c r="O9" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="P9" s="1" t="s">
+      <c r="P9" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="Q9" s="1" t="s">
+      <c r="Q9" s="3" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A10" s="1"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A11" s="1"/>
+      <c r="W11" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>